<commit_message>
Menambahkan file baru, menghapus file, dan memperbarui file yang diubah
</commit_message>
<xml_diff>
--- a/data_absensi_2024-09-21.xlsx
+++ b/data_absensi_2024-09-21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -841,6 +841,312 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>12225495</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>14:20:11</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>surya sahrul</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>3131</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>12c1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>14:21:38</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>surya sahrul</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1222549</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>12c1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>14:22:17</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>31312</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>12c1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>14:29:04</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Tidak Diketahui</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>313121</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>12c1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>14:29:57</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>31312</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>14:30:47</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>surya sahrul muhammad</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>313121</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>12c1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>14:31:39</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>122025495100</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>14:38:50</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>122032545100</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>14:38:50</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>12225495100</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>14:38:52</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0066944417</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>14:38:56</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>14:38:58</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0012</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>14:47:52</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>00133</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>14:48:17</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Terlambat</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>